<commit_message>
them history va options
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 3\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 4\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Username</t>
-  </si>
-  <si>
-    <t>;1</t>
   </si>
 </sst>
 </file>
@@ -412,9 +409,6 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chay duoc 1 man dua
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Username</t>
+  </si>
+  <si>
+    <t>minhkhoi</t>
   </si>
 </sst>
 </file>
@@ -353,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
@@ -410,6 +413,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1000</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chinh sua chon duong dua
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 4\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C955979-D4BD-4A4C-823C-16162D221F00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12130"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -355,20 +356,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -379,7 +380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -396,7 +397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -413,12 +414,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>1200</v>
       </c>
       <c r="C4">
         <v>0</v>

</xml_diff>

<commit_message>
hien thi lich su, (con loi lech set, nhan vat)
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -54,6 +54,15 @@
   </si>
   <si>
     <t>anhlavodich</t>
+  </si>
+  <si>
+    <t>;0;0</t>
+  </si>
+  <si>
+    <t>;13;23</t>
+  </si>
+  <si>
+    <t>;-1000;-98000.0</t>
   </si>
 </sst>
 </file>
@@ -518,16 +527,25 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>198000</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xe chay trong game giong xe da chon
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/22120221_student_hcmus_edu_vn/Documents/game/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="11_2CF6E75F0FA2EA7C115328EAF1186BF62BD265E5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CBBCF3A8-59F0-4BA5-A8C0-6026E8AA4545}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99D01CF-4763-427B-8450-04CA841DDBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -378,13 +378,13 @@
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -395,7 +395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -412,7 +412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -429,7 +429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -446,7 +446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -463,7 +463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -480,7 +480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -497,7 +497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -514,7 +514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
chỉnh 1 tí xíu
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>;-1000;-98000.0</t>
+  </si>
+  <si>
+    <t>;0</t>
+  </si>
+  <si>
+    <t>;21</t>
+  </si>
+  <si>
+    <t>;-1000</t>
+  </si>
+  <si>
+    <t>;1</t>
+  </si>
+  <si>
+    <t>;20</t>
+  </si>
+  <si>
+    <t>;+100</t>
   </si>
 </sst>
 </file>
@@ -383,7 +401,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,16 +449,25 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
@@ -448,16 +475,25 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
thêm hướng dẫn chơi
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 6\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D0BBE8-AEE8-4237-AD74-B790030509AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -55,12 +54,21 @@
   </si>
   <si>
     <t>anhlavodich</t>
+  </si>
+  <si>
+    <t>;0</t>
+  </si>
+  <si>
+    <t>;12</t>
+  </si>
+  <si>
+    <t>;-500</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -371,20 +379,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -395,7 +403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -412,7 +420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -429,7 +437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -446,7 +454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -463,7 +471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -480,7 +488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -497,7 +505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -514,21 +522,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
-        <v>198000</v>
+        <v>197500</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thêm biến vatpham = ...
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>vipvipvip</t>
   </si>
@@ -56,13 +56,16 @@
     <t>anhlavodich</t>
   </si>
   <si>
-    <t>;0</t>
-  </si>
-  <si>
-    <t>;12</t>
-  </si>
-  <si>
-    <t>;-500</t>
+    <t>;0;0;0;0;0;0</t>
+  </si>
+  <si>
+    <t>;12;41;24;24;13;44</t>
+  </si>
+  <si>
+    <t>;-500;-500;-500;-500;-1000;-1000</t>
+  </si>
+  <si>
+    <t>;1;2;3;4;2</t>
   </si>
 </sst>
 </file>
@@ -527,16 +530,16 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>197500</v>
+        <v>193100</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -546,6 +549,9 @@
       </c>
       <c r="H9" t="s">
         <v>12</v>
+      </c>
+      <c r="I9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix loi out game
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\game\main game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11B60539-05AB-47F5-872F-25524E50036B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D55E51A-D4A1-4E70-BD81-23B74BF0508E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Username</t>
   </si>
@@ -38,6 +38,21 @@
   </si>
   <si>
     <t>TungDo</t>
+  </si>
+  <si>
+    <t>;3;1;1;4</t>
+  </si>
+  <si>
+    <t>superprovip</t>
+  </si>
+  <si>
+    <t>;0</t>
+  </si>
+  <si>
+    <t>;32</t>
+  </si>
+  <si>
+    <t>;-750.0</t>
   </si>
 </sst>
 </file>
@@ -409,20 +424,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +448,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -450,7 +465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -467,12 +482,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -483,8 +498,11 @@
       <c r="E4" s="3">
         <v>0</v>
       </c>
+      <c r="I4" s="4" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -499,6 +517,32 @@
       </c>
       <c r="E5" s="3">
         <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2">
+        <v>750</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix chon do dai duong dua
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D55E51A-D4A1-4E70-BD81-23B74BF0508E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17179409-C6F1-43B3-92CC-E23595AF33E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -46,13 +46,13 @@
     <t>superprovip</t>
   </si>
   <si>
-    <t>;0</t>
-  </si>
-  <si>
-    <t>;32</t>
-  </si>
-  <si>
-    <t>;-750.0</t>
+    <t>;0;0;0;0;0;0</t>
+  </si>
+  <si>
+    <t>;32;42;42;42;42;43</t>
+  </si>
+  <si>
+    <t>;-750.0;-100;-100;-100;-100;-100</t>
   </si>
 </sst>
 </file>
@@ -524,16 +524,16 @@
         <v>7</v>
       </c>
       <c r="B6" s="2">
-        <v>750</v>
+        <v>250</v>
       </c>
       <c r="C6" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
sửa lịch sử một chút
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 6\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C135C8-8F52-4FF2-BB8C-9024AB7DBB5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2690" yWindow="2690" windowWidth="17280" windowHeight="8960"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="31">
   <si>
     <t>Username</t>
   </si>
@@ -92,12 +91,33 @@
   </si>
   <si>
     <t>;-100;-200;-100;+600;+700</t>
+  </si>
+  <si>
+    <t>Số trận đấu</t>
+  </si>
+  <si>
+    <t>Số lần thắng</t>
+  </si>
+  <si>
+    <t>Số lần thua</t>
+  </si>
+  <si>
+    <t>Lịch sử đấu (Thắng-1/Thua-0)</t>
+  </si>
+  <si>
+    <t>;1;1</t>
+  </si>
+  <si>
+    <t>;22;23</t>
+  </si>
+  <si>
+    <t>;+100;+100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,33 +479,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.21875" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="G1" t="s">
         <v>8</v>
       </c>
@@ -496,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -513,7 +546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -539,7 +572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -565,7 +598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -582,24 +615,33 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2000</v>
+        <v>2200</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <v>0</v>
       </c>
+      <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -628,7 +670,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -652,9 +694,6 @@
       </c>
       <c r="H8" t="s">
         <v>20</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tinh tien cho minigame
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\game\main game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 6\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246ED342-9D6E-4906-B8E5-2376B7D1172C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="15380" windowHeight="8330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Username</t>
   </si>
@@ -106,15 +105,6 @@
     <t>Lịch sử đấu (Thắng-1/Thua-0)</t>
   </si>
   <si>
-    <t>;1;1</t>
-  </si>
-  <si>
-    <t>;22;23</t>
-  </si>
-  <si>
-    <t>;+100;+100</t>
-  </si>
-  <si>
     <t>;0;0;0;0;0;0</t>
   </si>
   <si>
@@ -122,12 +112,33 @@
   </si>
   <si>
     <t>;-100;-400.0;-400.0;-215.0;-215.0;-100</t>
+  </si>
+  <si>
+    <t>;1;1;0;0;0;1;0;0</t>
+  </si>
+  <si>
+    <t>;22;23;43;22;41;30;30;24</t>
+  </si>
+  <si>
+    <t>;+100;+100;-2200;-200;-1000;+100;-250;-100</t>
+  </si>
+  <si>
+    <t>accmoii</t>
+  </si>
+  <si>
+    <t>;0;0;1</t>
+  </si>
+  <si>
+    <t>;14;33;13</t>
+  </si>
+  <si>
+    <t>;-120.0;-120;+50.0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -188,6 +199,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,28 +501,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.1796875" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.1796875" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -539,7 +551,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -556,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -582,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -608,7 +620,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -625,42 +637,42 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2200</v>
+        <v>30</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D6" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -689,7 +701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -714,6 +726,35 @@
       <c r="H8" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2">
+        <v>150</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix bug lịch sử
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -126,13 +126,13 @@
     <t>accmoii</t>
   </si>
   <si>
-    <t>;0;0;1</t>
-  </si>
-  <si>
-    <t>;14;33;13</t>
-  </si>
-  <si>
-    <t>;-120.0;-120;+50.0</t>
+    <t>;0;0;1;1;0;1;0;0;0</t>
+  </si>
+  <si>
+    <t>;14;33;13;13;10;13;31;0;4</t>
+  </si>
+  <si>
+    <t>;-120.0;-120;+50.0;+100;-100;+1499700;-1499700;-1499700;-100</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>30</v>
+        <v>210</v>
       </c>
       <c r="C6" s="2">
         <v>8</v>
@@ -732,16 +732,16 @@
         <v>34</v>
       </c>
       <c r="B9" s="2">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2">
+        <v>9</v>
+      </c>
+      <c r="D9" s="2">
         <v>3</v>
       </c>
-      <c r="D9" s="2">
-        <v>1</v>
-      </c>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
chinh full screen luc dua xe
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 6\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E5F082-C90B-443D-AA3C-88A9FA5270E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="15380" windowHeight="8330"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,15 +85,6 @@
     <t>;-200;-500</t>
   </si>
   <si>
-    <t>;0;0;0;1;1</t>
-  </si>
-  <si>
-    <t>;0;0;0;0;3</t>
-  </si>
-  <si>
-    <t>;-100;-200;-100;+600;+700</t>
-  </si>
-  <si>
     <t>Số trận đấu</t>
   </si>
   <si>
@@ -133,12 +125,21 @@
   </si>
   <si>
     <t>;-120.0;-120;+50.0;+100;-100;+1499700;-1499700;-1499700;-100</t>
+  </si>
+  <si>
+    <t>;0;0;0;1;1;0</t>
+  </si>
+  <si>
+    <t>;0;0;0;0;3;42</t>
+  </si>
+  <si>
+    <t>;-100;-200;-100;+600;+700;-200</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -501,7 +502,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -511,18 +512,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.1796875" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.1796875" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.21875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.21875" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,16 +531,16 @@
         <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="G1" t="s">
         <v>8</v>
@@ -551,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -568,7 +569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -594,33 +595,33 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>1400</v>
+        <v>600</v>
       </c>
       <c r="C4" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="H4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -637,16 +638,16 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -663,16 +664,16 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -701,7 +702,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -727,9 +728,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B9" s="2">
         <v>50</v>
@@ -744,16 +745,16 @@
         <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="H9" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="E15" s="5"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sua loi mua do
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\game\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\study\NMLT\game\game\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0924ACEE-94F0-40C8-B46C-CFC1AC3A5E1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B8DC5F-CF1E-46C3-8335-4BB1175D2416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="15375" windowHeight="8325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -109,15 +109,6 @@
     <t>accmoii</t>
   </si>
   <si>
-    <t>;0;0;0;1;1;0</t>
-  </si>
-  <si>
-    <t>;0;0;0;0;3;42</t>
-  </si>
-  <si>
-    <t>;-100;-200;-100;+600;+700;-200</t>
-  </si>
-  <si>
     <t>;0;0;1;1;0;1;0;0;0;0;0</t>
   </si>
   <si>
@@ -146,6 +137,18 @@
   </si>
   <si>
     <t>;-100;-400.0;-400.0;-215.0;-215.0;-100;-100</t>
+  </si>
+  <si>
+    <t>;2;2</t>
+  </si>
+  <si>
+    <t>;0;0;0;1;1;0;0;0;0;0;0</t>
+  </si>
+  <si>
+    <t>;0;0;0;0;3;42;33;31;0;42;43</t>
+  </si>
+  <si>
+    <t>;-100;-200;-100;+600;+700;-200;-500;-100;-120;-100;-220</t>
   </si>
 </sst>
 </file>
@@ -524,18 +527,18 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,7 +567,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -581,7 +584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -607,33 +610,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>600</v>
+        <v>0</v>
       </c>
       <c r="C4" s="3">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
       </c>
       <c r="E4" s="3">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -650,16 +656,16 @@
         <v>7</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -685,7 +691,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -714,7 +720,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -740,7 +746,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -757,21 +763,21 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>32</v>
-      </c>
-      <c r="G9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
       </c>
       <c r="B16" s="2">
         <v>140</v>
@@ -789,15 +795,15 @@
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B17" s="2">
         <v>0</v>

</xml_diff>

<commit_message>
thêm credit, chỉnh một số hiệu ứng nút
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -141,16 +141,13 @@
     <t>;-100;-200;-100;+600;+700;-200;-500;-100;-120;-100;-220</t>
   </si>
   <si>
-    <t>;0;0;1;1;0;1;0;0;0;0;0;0;0;0</t>
-  </si>
-  <si>
-    <t>;14;33;13;13;10;13;31;0;4;42;0;0;0;0</t>
-  </si>
-  <si>
-    <t>;-120.0;-120;+50.0;+100;-100;+1499700;-1499700;-1499700;-100;-100;-100;-120;-100;-100</t>
-  </si>
-  <si>
-    <t>;2;2;2;2;2</t>
+    <t>;0;0;1;1;0;1;0;0;0;0;0;0;0;0;0;0;1;1;0;0;0;0</t>
+  </si>
+  <si>
+    <t>;14;33;13;13;10;13;31;0;4;42;0;0;0;0;0;3.0;3.0;43;31;3;44;0</t>
+  </si>
+  <si>
+    <t>;-120.0;-120;+50.0;+100;-100;+1499700;-1499700;-1499700;-100;-100;-100;-120;-100;-100;-100;-4999999500.0;+4999999500.0;+4999999100.0;-14999997000;-120;-120;-120</t>
   </si>
 </sst>
 </file>
@@ -205,11 +202,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -218,6 +212,18 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,46 +532,46 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.36328125" customWidth="1"/>
-    <col min="9" max="9" width="13.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33.26953125" customWidth="1"/>
+    <col min="8" max="8" width="76.453125" customWidth="1"/>
+    <col min="9" max="9" width="23.1796875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -573,16 +579,16 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <v>0</v>
-      </c>
-      <c r="C2" s="3">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3">
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2">
         <v>0</v>
       </c>
     </row>
@@ -590,16 +596,16 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1300</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>4</v>
       </c>
-      <c r="D3" s="3">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3">
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
         <v>4</v>
       </c>
       <c r="F3" t="s">
@@ -616,16 +622,16 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>11</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>2</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>9</v>
       </c>
       <c r="F4" t="s">
@@ -637,7 +643,7 @@
       <c r="H4" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="3" t="s">
         <v>36</v>
       </c>
     </row>
@@ -645,16 +651,16 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>130</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
         <v>7</v>
       </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
         <v>7</v>
       </c>
       <c r="F5" t="s">
@@ -671,16 +677,16 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>210</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>3</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>5</v>
       </c>
       <c r="F6" t="s">
@@ -697,16 +703,16 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1600</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
         <v>1</v>
       </c>
       <c r="F7" t="s">
@@ -718,7 +724,7 @@
       <c r="H7" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
@@ -726,16 +732,16 @@
       <c r="A8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>1100</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>2</v>
       </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
         <v>2</v>
       </c>
       <c r="F8" t="s">
@@ -752,17 +758,17 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2">
-        <v>80</v>
-      </c>
-      <c r="C9" s="2">
-        <v>14</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3</v>
-      </c>
-      <c r="E9" s="2">
-        <v>11</v>
+      <c r="B9" s="1">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1">
+        <v>22</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="1">
+        <v>17</v>
       </c>
       <c r="F9" t="s">
         <v>40</v>
@@ -773,27 +779,24 @@
       <c r="H9" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="4" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="E15" s="5"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>140</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>4</v>
       </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
         <v>4</v>
       </c>
       <c r="F16" t="s">
@@ -810,16 +813,16 @@
       <c r="A17" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2">
-        <v>0</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix AI auto cay khong
</commit_message>
<xml_diff>
--- a/data/userhistory.xlsx
+++ b/data/userhistory.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\version 6\game\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studenthcmusedu-my.sharepoint.com/personal/22120221_student_hcmus_edu_vn/Documents/game/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="39" documentId="11_C946C54B97E7CF0FE7606B43E72675AB4258DDCE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6312E44-914E-453E-8614-6B61FEF3C76D}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8960"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Username</t>
   </si>
@@ -148,12 +149,21 @@
   </si>
   <si>
     <t>;-120.0;-120;+50.0;+100;-100;+1499700;-1499700;-1499700;-100;-100;-100;-120;-100;-100;-100;-4999999500.0;+4999999500.0;+4999999100.0;-14999997000;-120;-120;-120</t>
+  </si>
+  <si>
+    <t>nam354</t>
+  </si>
+  <si>
+    <t>;1</t>
+  </si>
+  <si>
+    <t>;+100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -525,28 +535,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.36328125" customWidth="1"/>
-    <col min="7" max="7" width="33.26953125" customWidth="1"/>
-    <col min="8" max="8" width="76.453125" customWidth="1"/>
-    <col min="9" max="9" width="23.1796875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="33.28515625" customWidth="1"/>
+    <col min="8" max="8" width="76.42578125" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -575,7 +585,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -592,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -618,7 +628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -647,7 +657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -673,7 +683,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -699,7 +709,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -728,7 +738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -754,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -780,10 +790,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -809,7 +819,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -824,6 +834,32 @@
       </c>
       <c r="E17" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1">
+        <v>200</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>44</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>